<commit_message>
Exsel fixed more so
</commit_message>
<xml_diff>
--- a/Soil Teating.xlsx
+++ b/Soil Teating.xlsx
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G2:G106"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5292,7 +5292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>

</xml_diff>